<commit_message>
Modification de la documentation pour le rapport
</commit_message>
<xml_diff>
--- a/Documentation/ProximitySensors.xlsx
+++ b/Documentation/ProximitySensors.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\thibault.schaller\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\thibault.schaller\Desktop\TP_robotique\miniprojet_SlopeFollower\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9463C61-3548-4E9A-9311-64BF10E51C42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B97C007-A2D3-4623-A3EE-F57A47497BAD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12108" yWindow="816" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -144,6 +144,44 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="fr-CH" b="1"/>
+              <a:t>Valeur de</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="fr-CH" b="1" baseline="0"/>
+              <a:t> proximité en fonction de la distance</a:t>
+            </a:r>
+            <a:endParaRPr lang="fr-CH" b="1"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.17430555555555555"/>
+          <c:y val="4.1666666666666664E-2"/>
+        </c:manualLayout>
+      </c:layout>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -157,7 +195,7 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+            <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
               <a:solidFill>
                 <a:schemeClr val="tx1">
                   <a:lumMod val="65000"/>
@@ -346,6 +384,7 @@
         <c:axId val="1914101616"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="5"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
@@ -363,6 +402,61 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="fr-CH" b="1"/>
+                  <a:t>Distance [cm]</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="fr-FR"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -425,6 +519,69 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="fr-CH" b="1"/>
+                  <a:t>Valeur de proximité [-]</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout>
+            <c:manualLayout>
+              <c:xMode val="edge"/>
+              <c:yMode val="edge"/>
+              <c:x val="2.2222222222222223E-2"/>
+              <c:y val="0.25639289880431615"/>
+            </c:manualLayout>
+          </c:layout>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="fr-FR"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -1381,7 +1538,7 @@
   <dimension ref="A1:B25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+      <selection activeCell="M10" sqref="M10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>